<commit_message>
renamed:    "\347\254\254\344\270\200\347\253\240  \346\225\260\347\273\204part01 .docx" -> "1/\347\254\254\344\270\200\347\253\240  \346\225\260\347\273\204part01 .docx" 	modified:   "\347\273\237\350\256\241.xlsx"
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C48502A-8B74-4B0C-9504-9B4E86DADFDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02D774F-4D1E-4761-AB96-DB6BA1AA5764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>double ptr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>二分法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快慢指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -355,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -366,12 +378,15 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45301</v>
       </c>
@@ -381,11 +396,26 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3">
         <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>